<commit_message>
Results from July 06, 2020 12:20:25 AM run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
@@ -1796,7 +1796,7 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C28" t="n">
         <v>23814</v>
@@ -2286,13 +2286,13 @@
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C38" t="n">
-        <v>14553</v>
+        <v>14751</v>
       </c>
       <c r="D38" t="n">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E38" t="n">
         <v>464</v>

</xml_diff>

<commit_message>
Results from July 06, 2020 03:21:54 AM CT run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
@@ -518,51 +518,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44017</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>213852</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>18583</t>
-        </is>
+      <c r="C2" t="n">
+        <v>23133</v>
+      </c>
+      <c r="D2" t="n">
+        <v>680</v>
       </c>
       <c r="E2" t="n">
-        <v>33240</v>
+        <v>2710</v>
       </c>
       <c r="F2" t="n">
-        <v>5195</v>
+        <v>87</v>
       </c>
       <c r="G2" t="n">
-        <v>30.17</v>
+        <v>0.12</v>
       </c>
       <c r="H2" t="n">
-        <v>30.5</v>
+        <v>0.13</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>110192</v>
-      </c>
-      <c r="L2" t="n">
-        <v>17034</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>2049418</v>
+        <v>3365783</v>
       </c>
       <c r="N2" t="n">
-        <v>24.27</v>
+        <v>12.07</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -573,43 +565,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C3" t="n">
-        <v>109974</v>
+        <v>14751</v>
       </c>
       <c r="D3" t="n">
-        <v>8183</v>
+        <v>130</v>
       </c>
       <c r="E3" t="n">
-        <v>10357</v>
+        <v>464</v>
       </c>
       <c r="F3" t="n">
-        <v>669</v>
+        <v>17</v>
       </c>
       <c r="G3" t="n">
-        <v>9.42</v>
+        <v>6.81</v>
       </c>
       <c r="H3" t="n">
-        <v>8.18</v>
+        <v>15.32</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>6812</v>
+      </c>
+      <c r="L3" t="n">
+        <v>111</v>
+      </c>
       <c r="M3" t="n">
-        <v>510558</v>
+        <v>146703</v>
       </c>
       <c r="N3" t="n">
-        <v>7.48</v>
+        <v>7.62</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -620,47 +616,51 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
         <v>44017</v>
       </c>
-      <c r="C4" t="n">
-        <v>35898</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1359</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>213852</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18583</t>
+        </is>
       </c>
       <c r="E4" t="n">
-        <v>1436</v>
+        <v>33240</v>
       </c>
       <c r="F4" t="n">
-        <v>45</v>
+        <v>5195</v>
       </c>
       <c r="G4" t="n">
-        <v>5.49</v>
+        <v>30.17</v>
       </c>
       <c r="H4" t="n">
-        <v>3.46</v>
+        <v>30.5</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>26150</v>
+        <v>110192</v>
       </c>
       <c r="L4" t="n">
-        <v>1301</v>
+        <v>17034</v>
       </c>
       <c r="M4" t="n">
-        <v>269854</v>
+        <v>2049418</v>
       </c>
       <c r="N4" t="n">
-        <v>3.7</v>
+        <v>24.27</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -671,29 +671,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44017</v>
+        <v>44015</v>
       </c>
       <c r="C5" t="n">
-        <v>34065</v>
+        <v>16491</v>
       </c>
       <c r="D5" t="n">
-        <v>1701</v>
+        <v>960</v>
       </c>
       <c r="E5" t="n">
-        <v>1809</v>
+        <v>1592</v>
       </c>
       <c r="F5" t="n">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="G5" t="n">
-        <v>6.45</v>
+        <v>12.29</v>
       </c>
       <c r="H5" t="n">
-        <v>6.78</v>
+        <v>6.14</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -702,16 +702,16 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>28039</v>
+        <v>12950</v>
       </c>
       <c r="L5" t="n">
-        <v>1638</v>
+        <v>782</v>
       </c>
       <c r="M5" t="n">
-        <v>227938</v>
+        <v>69254</v>
       </c>
       <c r="N5" t="n">
-        <v>4.12</v>
+        <v>6.55</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -722,43 +722,43 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C6" t="n">
-        <v>197076</v>
+        <v>51431</v>
       </c>
       <c r="D6" t="n">
-        <v>3731</v>
+        <v>646</v>
       </c>
       <c r="E6" t="n">
-        <v>25942</v>
+        <v>10459</v>
       </c>
       <c r="F6" t="n">
-        <v>728</v>
+        <v>228</v>
       </c>
       <c r="G6" t="n">
-        <v>13.16</v>
+        <v>20.34</v>
       </c>
       <c r="H6" t="n">
-        <v>19.51</v>
+        <v>35.29</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
-        <v>3316376</v>
+        <v>1117489</v>
       </c>
       <c r="N6" t="n">
-        <v>16.1</v>
+        <v>16.8</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -769,41 +769,49 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
         <v>44017</v>
       </c>
-      <c r="C7" t="n">
-        <v>3415</v>
-      </c>
-      <c r="D7" t="n">
-        <v>120</v>
-      </c>
-      <c r="E7" t="n">
-        <v>803</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24952</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
+      </c>
       <c r="G7" t="n">
-        <v>26.65</v>
+        <v>2.6</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3013</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>17881</v>
+        <v>35862</v>
       </c>
       <c r="N7" t="n">
-        <v>1.34</v>
+        <v>1.18</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -814,29 +822,29 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Idaho</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44017</v>
+        <v>44015</v>
       </c>
       <c r="C8" t="n">
-        <v>7733</v>
+        <v>16376</v>
       </c>
       <c r="D8" t="n">
-        <v>92</v>
+        <v>585</v>
       </c>
       <c r="E8" t="n">
-        <v>114</v>
+        <v>1607</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="G8" t="n">
-        <v>1.47</v>
+        <v>14.06</v>
       </c>
       <c r="H8" t="n">
-        <v>1.09</v>
+        <v>15.72</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -844,13 +852,17 @@
       <c r="J8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>11432</v>
+      </c>
+      <c r="L8" t="n">
+        <v>546</v>
+      </c>
       <c r="M8" t="n">
-        <v>11536</v>
+        <v>354112</v>
       </c>
       <c r="N8" t="n">
-        <v>0.68</v>
+        <v>7.98</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -861,43 +873,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C9" t="n">
-        <v>95516</v>
+        <v>23814</v>
       </c>
       <c r="D9" t="n">
-        <v>2860</v>
+        <v>287</v>
       </c>
       <c r="E9" t="n">
-        <v>26475</v>
+        <v>5169</v>
       </c>
       <c r="F9" t="n">
-        <v>1352</v>
+        <v>70</v>
       </c>
       <c r="G9" t="n">
-        <v>27.72</v>
+        <v>25.26</v>
       </c>
       <c r="H9" t="n">
-        <v>47.27</v>
+        <v>25.55</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>20467</v>
+      </c>
+      <c r="L9" t="n">
+        <v>274</v>
+      </c>
       <c r="M9" t="n">
-        <v>3239300</v>
+        <v>460970</v>
       </c>
       <c r="N9" t="n">
-        <v>31.46</v>
+        <v>15.41</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -908,43 +924,47 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>California - San Diego</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44015</v>
+        <v>44017</v>
       </c>
       <c r="C10" t="n">
-        <v>30674</v>
+        <v>16726</v>
       </c>
       <c r="D10" t="n">
-        <v>1107</v>
+        <v>387</v>
       </c>
       <c r="E10" t="n">
-        <v>14869</v>
+        <v>606</v>
       </c>
       <c r="F10" t="n">
-        <v>553</v>
+        <v>13</v>
       </c>
       <c r="G10" t="n">
-        <v>48.47</v>
+        <v>4.56</v>
       </c>
       <c r="H10" t="n">
-        <v>49.95</v>
+        <v>3.4</v>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>13303</v>
+      </c>
+      <c r="L10" t="n">
+        <v>382</v>
+      </c>
       <c r="M10" t="n">
-        <v>1125834</v>
+        <v>166412</v>
       </c>
       <c r="N10" t="n">
-        <v>37.67</v>
+        <v>5.04</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -955,47 +975,43 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44013</v>
+        <v>44017</v>
       </c>
       <c r="C11" t="n">
-        <v>107667</v>
+        <v>65748</v>
       </c>
       <c r="D11" t="n">
-        <v>3454</v>
+        <v>1853</v>
       </c>
       <c r="E11" t="n">
-        <v>2946</v>
+        <v>9541</v>
       </c>
       <c r="F11" t="n">
-        <v>365</v>
+        <v>413</v>
       </c>
       <c r="G11" t="n">
-        <v>4.6</v>
+        <v>14.51</v>
       </c>
       <c r="H11" t="n">
-        <v>11.37</v>
+        <v>22.29</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>63985</v>
-      </c>
-      <c r="L11" t="n">
-        <v>3209</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>823987</v>
+        <v>1613285</v>
       </c>
       <c r="N11" t="n">
-        <v>8.16</v>
+        <v>19.17</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1006,34 +1022,24 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
         <v>44017</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>24952</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>184</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>654</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>&lt;5</t>
-        </is>
-      </c>
+      <c r="C12" t="n">
+        <v>13256</v>
+      </c>
+      <c r="D12" t="n">
+        <v>513</v>
+      </c>
+      <c r="E12" t="n">
+        <v>256</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>2.6</v>
+        <v>1.93</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="b">
@@ -1045,10 +1051,10 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
-        <v>35862</v>
+        <v>43006</v>
       </c>
       <c r="N12" t="n">
-        <v>1.18</v>
+        <v>2.06</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1059,47 +1065,41 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C13" t="n">
-        <v>12213</v>
+        <v>47011</v>
       </c>
       <c r="D13" t="n">
-        <v>355</v>
+        <v>1043</v>
       </c>
       <c r="E13" t="n">
-        <v>3517</v>
-      </c>
-      <c r="F13" t="n">
-        <v>143</v>
-      </c>
+        <v>5798</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>31.08</v>
-      </c>
-      <c r="H13" t="n">
-        <v>40.28</v>
-      </c>
+        <v>21.01</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>11317</v>
-      </c>
-      <c r="L13" t="n">
-        <v>355</v>
-      </c>
+        <v>27600</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>252321</v>
+        <v>481976</v>
       </c>
       <c r="N13" t="n">
-        <v>26.44</v>
+        <v>17.75</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1110,43 +1110,41 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C14" t="n">
-        <v>23133</v>
+        <v>14032</v>
       </c>
       <c r="D14" t="n">
-        <v>680</v>
+        <v>59</v>
       </c>
       <c r="E14" t="n">
-        <v>2710</v>
-      </c>
-      <c r="F14" t="n">
-        <v>87</v>
-      </c>
+        <v>1780</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.13</v>
-      </c>
+        <v>23.96</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>7430</v>
+      </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>3365783</v>
+        <v>277193</v>
       </c>
       <c r="N14" t="n">
-        <v>12.07</v>
+        <v>20.98</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1157,47 +1155,47 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44009</v>
+        <v>44017</v>
       </c>
       <c r="C15" t="n">
-        <v>20261</v>
+        <v>43450</v>
       </c>
       <c r="D15" t="n">
-        <v>996</v>
+        <v>984</v>
       </c>
       <c r="E15" t="n">
-        <v>5758</v>
+        <v>15319</v>
       </c>
       <c r="F15" t="n">
-        <v>246</v>
+        <v>442</v>
       </c>
       <c r="G15" t="n">
-        <v>49.66</v>
+        <v>46.59</v>
       </c>
       <c r="H15" t="n">
-        <v>38.56</v>
+        <v>46.48</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>11594</v>
+        <v>32881</v>
       </c>
       <c r="L15" t="n">
-        <v>638</v>
+        <v>951</v>
       </c>
       <c r="M15" t="n">
-        <v>704896</v>
+        <v>1293186</v>
       </c>
       <c r="N15" t="n">
-        <v>11.57</v>
+        <v>26.58</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1208,43 +1206,47 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>California - Los Angeles</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44017</v>
+        <v>44013</v>
       </c>
       <c r="C16" t="n">
-        <v>65748</v>
+        <v>107667</v>
       </c>
       <c r="D16" t="n">
-        <v>1853</v>
+        <v>3454</v>
       </c>
       <c r="E16" t="n">
-        <v>9541</v>
+        <v>2946</v>
       </c>
       <c r="F16" t="n">
-        <v>413</v>
+        <v>365</v>
       </c>
       <c r="G16" t="n">
-        <v>14.51</v>
+        <v>4.6</v>
       </c>
       <c r="H16" t="n">
-        <v>22.29</v>
+        <v>11.37</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>63985</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3209</v>
+      </c>
       <c r="M16" t="n">
-        <v>1613285</v>
+        <v>823987</v>
       </c>
       <c r="N16" t="n">
-        <v>19.17</v>
+        <v>8.16</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1255,29 +1257,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44015</v>
+        <v>44017</v>
       </c>
       <c r="C17" t="n">
-        <v>16491</v>
+        <v>69632</v>
       </c>
       <c r="D17" t="n">
-        <v>960</v>
+        <v>3118</v>
       </c>
       <c r="E17" t="n">
-        <v>1592</v>
+        <v>19953</v>
       </c>
       <c r="F17" t="n">
-        <v>48</v>
+        <v>1258</v>
       </c>
       <c r="G17" t="n">
-        <v>12.29</v>
+        <v>28.65</v>
       </c>
       <c r="H17" t="n">
-        <v>6.14</v>
+        <v>40.35</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1286,16 +1288,16 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>12950</v>
+        <v>57047</v>
       </c>
       <c r="L17" t="n">
-        <v>782</v>
+        <v>69602</v>
       </c>
       <c r="M17" t="n">
-        <v>69254</v>
+        <v>1788090</v>
       </c>
       <c r="N17" t="n">
-        <v>6.55</v>
+        <v>29.78</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1306,29 +1308,29 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44017</v>
+        <v>44015</v>
       </c>
       <c r="C18" t="n">
-        <v>10482</v>
+        <v>30674</v>
       </c>
       <c r="D18" t="n">
-        <v>559</v>
+        <v>1107</v>
       </c>
       <c r="E18" t="n">
-        <v>5213</v>
+        <v>14869</v>
       </c>
       <c r="F18" t="n">
-        <v>412</v>
+        <v>553</v>
       </c>
       <c r="G18" t="n">
-        <v>49.73</v>
+        <v>48.47</v>
       </c>
       <c r="H18" t="n">
-        <v>73.7</v>
+        <v>49.95</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -1339,10 +1341,10 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>321317</v>
+        <v>1125834</v>
       </c>
       <c r="N18" t="n">
-        <v>46.94</v>
+        <v>37.67</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1353,43 +1355,47 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C19" t="n">
-        <v>12128</v>
+        <v>87267</v>
       </c>
       <c r="D19" t="n">
-        <v>512</v>
+        <v>6753</v>
       </c>
       <c r="E19" t="n">
-        <v>3124</v>
+        <v>11551</v>
       </c>
       <c r="F19" t="n">
-        <v>131</v>
+        <v>1426</v>
       </c>
       <c r="G19" t="n">
-        <v>25.76</v>
+        <v>30.05</v>
       </c>
       <c r="H19" t="n">
-        <v>25.59</v>
+        <v>21.68</v>
       </c>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>38441</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6579</v>
+      </c>
       <c r="M19" t="n">
-        <v>209892</v>
+        <v>1423319</v>
       </c>
       <c r="N19" t="n">
-        <v>22.11</v>
+        <v>11.13</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -1400,47 +1406,43 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C20" t="n">
-        <v>43450</v>
+        <v>197076</v>
       </c>
       <c r="D20" t="n">
-        <v>984</v>
+        <v>3731</v>
       </c>
       <c r="E20" t="n">
-        <v>15319</v>
+        <v>25942</v>
       </c>
       <c r="F20" t="n">
-        <v>442</v>
+        <v>728</v>
       </c>
       <c r="G20" t="n">
-        <v>46.59</v>
+        <v>13.16</v>
       </c>
       <c r="H20" t="n">
-        <v>46.48</v>
+        <v>19.51</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
       </c>
-      <c r="K20" t="n">
-        <v>32881</v>
-      </c>
-      <c r="L20" t="n">
-        <v>951</v>
-      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>1293186</v>
+        <v>3316376</v>
       </c>
       <c r="N20" t="n">
-        <v>26.58</v>
+        <v>16.1</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1451,39 +1453,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C21" t="n">
-        <v>13256</v>
+        <v>1212</v>
       </c>
       <c r="D21" t="n">
-        <v>513</v>
+        <v>23</v>
       </c>
       <c r="E21" t="n">
-        <v>256</v>
+        <v>6</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>1.93</v>
+        <v>0.5</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>43006</v>
+        <v>4630</v>
       </c>
       <c r="N21" t="n">
-        <v>2.06</v>
+        <v>0.44</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1545,47 +1547,47 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C23" t="n">
-        <v>87267</v>
+        <v>34065</v>
       </c>
       <c r="D23" t="n">
-        <v>6753</v>
+        <v>1701</v>
       </c>
       <c r="E23" t="n">
-        <v>11551</v>
+        <v>1809</v>
       </c>
       <c r="F23" t="n">
-        <v>1426</v>
+        <v>111</v>
       </c>
       <c r="G23" t="n">
-        <v>30.05</v>
+        <v>6.45</v>
       </c>
       <c r="H23" t="n">
-        <v>21.68</v>
+        <v>6.78</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>38441</v>
+        <v>28039</v>
       </c>
       <c r="L23" t="n">
-        <v>6579</v>
+        <v>1638</v>
       </c>
       <c r="M23" t="n">
-        <v>1423319</v>
+        <v>227938</v>
       </c>
       <c r="N23" t="n">
-        <v>11.13</v>
+        <v>4.12</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1596,43 +1598,47 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C24" t="n">
-        <v>147251</v>
+        <v>19929</v>
       </c>
       <c r="D24" t="n">
-        <v>7020</v>
+        <v>284</v>
       </c>
       <c r="E24" t="n">
-        <v>24691</v>
+        <v>1180</v>
       </c>
       <c r="F24" t="n">
-        <v>1958</v>
+        <v>21</v>
       </c>
       <c r="G24" t="n">
-        <v>16.77</v>
+        <v>7.66</v>
       </c>
       <c r="H24" t="n">
-        <v>27.89</v>
+        <v>7.72</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>15406</v>
+      </c>
+      <c r="L24" t="n">
+        <v>272</v>
+      </c>
       <c r="M24" t="n">
-        <v>1824125</v>
+        <v>90860</v>
       </c>
       <c r="N24" t="n">
-        <v>14.23</v>
+        <v>4.77</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1690,29 +1696,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44017</v>
+        <v>44016</v>
       </c>
       <c r="C26" t="n">
-        <v>1138</v>
+        <v>260155</v>
       </c>
       <c r="D26" t="n">
-        <v>16</v>
+        <v>6264</v>
       </c>
       <c r="E26" t="n">
-        <v>25</v>
+        <v>7432</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>572</v>
       </c>
       <c r="G26" t="n">
-        <v>1.26</v>
+        <v>4.3</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1721,16 +1727,16 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>1982</v>
+        <v>171792</v>
       </c>
       <c r="L26" t="n">
-        <v>32</v>
+        <v>6163</v>
       </c>
       <c r="M26" t="n">
-        <v>24129</v>
+        <v>2267875</v>
       </c>
       <c r="N26" t="n">
-        <v>3.27</v>
+        <v>5.79</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1741,47 +1747,43 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="C27" t="n">
-        <v>260155</v>
+        <v>48008</v>
       </c>
       <c r="D27" t="n">
-        <v>6264</v>
+        <v>2500</v>
       </c>
       <c r="E27" t="n">
-        <v>7432</v>
+        <v>5769</v>
       </c>
       <c r="F27" t="n">
-        <v>572</v>
+        <v>362</v>
       </c>
       <c r="G27" t="n">
-        <v>4.3</v>
+        <v>12.02</v>
       </c>
       <c r="H27" t="n">
-        <v>9.300000000000001</v>
+        <v>14.48</v>
       </c>
       <c r="I27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="b">
         <v>1</v>
       </c>
-      <c r="K27" t="n">
-        <v>171792</v>
-      </c>
-      <c r="L27" t="n">
-        <v>6163</v>
-      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
-        <v>2267875</v>
+        <v>619472</v>
       </c>
       <c r="N27" t="n">
-        <v>5.79</v>
+        <v>9.33</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1792,29 +1794,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44018</v>
+        <v>44017</v>
       </c>
       <c r="C28" t="n">
-        <v>23814</v>
+        <v>1138</v>
       </c>
       <c r="D28" t="n">
-        <v>287</v>
+        <v>16</v>
       </c>
       <c r="E28" t="n">
-        <v>5169</v>
+        <v>25</v>
       </c>
       <c r="F28" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>25.26</v>
+        <v>1.26</v>
       </c>
       <c r="H28" t="n">
-        <v>25.55</v>
+        <v>0</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -1823,16 +1825,16 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>20467</v>
+        <v>1982</v>
       </c>
       <c r="L28" t="n">
-        <v>274</v>
+        <v>32</v>
       </c>
       <c r="M28" t="n">
-        <v>460970</v>
+        <v>24129</v>
       </c>
       <c r="N28" t="n">
-        <v>15.41</v>
+        <v>3.27</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1843,47 +1845,47 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C29" t="n">
-        <v>69632</v>
+        <v>31577</v>
       </c>
       <c r="D29" t="n">
-        <v>3118</v>
+        <v>796</v>
       </c>
       <c r="E29" t="n">
-        <v>19953</v>
+        <v>5412</v>
       </c>
       <c r="F29" t="n">
-        <v>1258</v>
+        <v>188</v>
       </c>
       <c r="G29" t="n">
-        <v>28.65</v>
+        <v>19.08</v>
       </c>
       <c r="H29" t="n">
-        <v>40.35</v>
+        <v>23.95</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>57047</v>
+        <v>28371</v>
       </c>
       <c r="L29" t="n">
-        <v>69602</v>
+        <v>785</v>
       </c>
       <c r="M29" t="n">
-        <v>1788090</v>
+        <v>368744</v>
       </c>
       <c r="N29" t="n">
-        <v>29.78</v>
+        <v>6.38</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1894,47 +1896,43 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C30" t="n">
-        <v>16726</v>
+        <v>95516</v>
       </c>
       <c r="D30" t="n">
-        <v>387</v>
+        <v>2860</v>
       </c>
       <c r="E30" t="n">
-        <v>606</v>
+        <v>26475</v>
       </c>
       <c r="F30" t="n">
-        <v>13</v>
+        <v>1352</v>
       </c>
       <c r="G30" t="n">
-        <v>4.56</v>
+        <v>27.72</v>
       </c>
       <c r="H30" t="n">
-        <v>3.4</v>
+        <v>47.27</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" t="n">
-        <v>13303</v>
-      </c>
-      <c r="L30" t="n">
-        <v>382</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
-        <v>166412</v>
+        <v>3239300</v>
       </c>
       <c r="N30" t="n">
-        <v>5.04</v>
+        <v>31.46</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1945,43 +1943,47 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C31" t="n">
-        <v>38136</v>
+        <v>35898</v>
       </c>
       <c r="D31" t="n">
-        <v>1471</v>
+        <v>1359</v>
       </c>
       <c r="E31" t="n">
-        <v>7861</v>
+        <v>1436</v>
       </c>
       <c r="F31" t="n">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="G31" t="n">
-        <v>20.61</v>
+        <v>5.49</v>
       </c>
       <c r="H31" t="n">
-        <v>8.5</v>
+        <v>3.46</v>
       </c>
       <c r="I31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>26150</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1301</v>
+      </c>
       <c r="M31" t="n">
-        <v>342186</v>
+        <v>269854</v>
       </c>
       <c r="N31" t="n">
-        <v>6.19</v>
+        <v>3.7</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1992,47 +1994,43 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C32" t="n">
-        <v>19929</v>
+        <v>10482</v>
       </c>
       <c r="D32" t="n">
-        <v>284</v>
+        <v>559</v>
       </c>
       <c r="E32" t="n">
-        <v>1180</v>
+        <v>5213</v>
       </c>
       <c r="F32" t="n">
-        <v>21</v>
+        <v>412</v>
       </c>
       <c r="G32" t="n">
-        <v>7.66</v>
+        <v>49.73</v>
       </c>
       <c r="H32" t="n">
-        <v>7.72</v>
+        <v>73.7</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
       </c>
-      <c r="K32" t="n">
-        <v>15406</v>
-      </c>
-      <c r="L32" t="n">
-        <v>272</v>
-      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
-        <v>90860</v>
+        <v>321317</v>
       </c>
       <c r="N32" t="n">
-        <v>4.77</v>
+        <v>46.94</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2043,41 +2041,43 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C33" t="n">
-        <v>47011</v>
+        <v>12128</v>
       </c>
       <c r="D33" t="n">
-        <v>1043</v>
+        <v>512</v>
       </c>
       <c r="E33" t="n">
-        <v>5798</v>
-      </c>
-      <c r="F33" t="inlineStr"/>
+        <v>3124</v>
+      </c>
+      <c r="F33" t="n">
+        <v>131</v>
+      </c>
       <c r="G33" t="n">
-        <v>21.01</v>
-      </c>
-      <c r="H33" t="inlineStr"/>
+        <v>25.76</v>
+      </c>
+      <c r="H33" t="n">
+        <v>25.59</v>
+      </c>
       <c r="I33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
-        <v>27600</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="n">
-        <v>481976</v>
+        <v>209892</v>
       </c>
       <c r="N33" t="n">
-        <v>17.75</v>
+        <v>22.11</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2088,24 +2088,24 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C34" t="n">
-        <v>14032</v>
+        <v>3415</v>
       </c>
       <c r="D34" t="n">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="E34" t="n">
-        <v>1780</v>
+        <v>803</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>23.96</v>
+        <v>26.65</v>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="b">
@@ -2115,14 +2115,14 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>7430</v>
+        <v>3013</v>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>277193</v>
+        <v>17881</v>
       </c>
       <c r="N34" t="n">
-        <v>20.98</v>
+        <v>1.34</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2133,29 +2133,29 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44015</v>
+        <v>44017</v>
       </c>
       <c r="C35" t="n">
-        <v>16376</v>
+        <v>72983</v>
       </c>
       <c r="D35" t="n">
-        <v>585</v>
+        <v>1396</v>
       </c>
       <c r="E35" t="n">
-        <v>1607</v>
+        <v>11722</v>
       </c>
       <c r="F35" t="n">
-        <v>85</v>
+        <v>445</v>
       </c>
       <c r="G35" t="n">
-        <v>14.06</v>
+        <v>23.71</v>
       </c>
       <c r="H35" t="n">
-        <v>15.72</v>
+        <v>33.04</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -2164,16 +2164,16 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>11432</v>
+        <v>49433</v>
       </c>
       <c r="L35" t="n">
-        <v>546</v>
+        <v>1347</v>
       </c>
       <c r="M35" t="n">
-        <v>354112</v>
+        <v>2179622</v>
       </c>
       <c r="N35" t="n">
-        <v>7.98</v>
+        <v>21.46</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2184,47 +2184,43 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C36" t="n">
-        <v>72983</v>
+        <v>147251</v>
       </c>
       <c r="D36" t="n">
-        <v>1396</v>
+        <v>7020</v>
       </c>
       <c r="E36" t="n">
-        <v>11722</v>
+        <v>24691</v>
       </c>
       <c r="F36" t="n">
-        <v>445</v>
+        <v>1958</v>
       </c>
       <c r="G36" t="n">
-        <v>23.71</v>
+        <v>16.77</v>
       </c>
       <c r="H36" t="n">
-        <v>33.04</v>
+        <v>27.89</v>
       </c>
       <c r="I36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36" t="n">
-        <v>49433</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1347</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
-        <v>2179622</v>
+        <v>1824125</v>
       </c>
       <c r="N36" t="n">
-        <v>21.46</v>
+        <v>14.23</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2235,32 +2231,32 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C37" t="n">
-        <v>48008</v>
+        <v>7733</v>
       </c>
       <c r="D37" t="n">
-        <v>2500</v>
+        <v>92</v>
       </c>
       <c r="E37" t="n">
-        <v>5769</v>
+        <v>114</v>
       </c>
       <c r="F37" t="n">
-        <v>362</v>
+        <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>12.02</v>
+        <v>1.47</v>
       </c>
       <c r="H37" t="n">
-        <v>14.48</v>
+        <v>1.09</v>
       </c>
       <c r="I37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="b">
         <v>1</v>
@@ -2268,10 +2264,10 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="n">
-        <v>619472</v>
+        <v>11536</v>
       </c>
       <c r="N37" t="n">
-        <v>9.33</v>
+        <v>0.68</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2282,47 +2278,43 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44018</v>
+        <v>44017</v>
       </c>
       <c r="C38" t="n">
-        <v>14751</v>
+        <v>38136</v>
       </c>
       <c r="D38" t="n">
-        <v>130</v>
+        <v>1471</v>
       </c>
       <c r="E38" t="n">
-        <v>464</v>
+        <v>7861</v>
       </c>
       <c r="F38" t="n">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="G38" t="n">
-        <v>6.81</v>
+        <v>20.61</v>
       </c>
       <c r="H38" t="n">
-        <v>15.32</v>
+        <v>8.5</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
-        <v>6812</v>
-      </c>
-      <c r="L38" t="n">
-        <v>111</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
-        <v>146703</v>
+        <v>342186</v>
       </c>
       <c r="N38" t="n">
-        <v>7.62</v>
+        <v>6.19</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2333,39 +2325,43 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C39" t="n">
-        <v>1212</v>
+        <v>109974</v>
       </c>
       <c r="D39" t="n">
-        <v>23</v>
+        <v>8183</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
+        <v>10357</v>
+      </c>
+      <c r="F39" t="n">
+        <v>669</v>
+      </c>
       <c r="G39" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H39" t="inlineStr"/>
+        <v>9.42</v>
+      </c>
+      <c r="H39" t="n">
+        <v>8.18</v>
+      </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="n">
-        <v>4630</v>
+        <v>510558</v>
       </c>
       <c r="N39" t="n">
-        <v>0.44</v>
+        <v>7.48</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2376,47 +2372,47 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
         <v>44017</v>
       </c>
       <c r="C40" t="n">
-        <v>31577</v>
+        <v>12213</v>
       </c>
       <c r="D40" t="n">
-        <v>796</v>
+        <v>355</v>
       </c>
       <c r="E40" t="n">
-        <v>5412</v>
+        <v>3517</v>
       </c>
       <c r="F40" t="n">
-        <v>188</v>
+        <v>143</v>
       </c>
       <c r="G40" t="n">
-        <v>19.08</v>
+        <v>31.08</v>
       </c>
       <c r="H40" t="n">
-        <v>23.95</v>
+        <v>40.28</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
       <c r="J40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>28371</v>
+        <v>11317</v>
       </c>
       <c r="L40" t="n">
-        <v>785</v>
+        <v>355</v>
       </c>
       <c r="M40" t="n">
-        <v>368744</v>
+        <v>252321</v>
       </c>
       <c r="N40" t="n">
-        <v>6.38</v>
+        <v>26.44</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2427,43 +2423,47 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44017</v>
+        <v>44009</v>
       </c>
       <c r="C41" t="n">
-        <v>51431</v>
+        <v>20261</v>
       </c>
       <c r="D41" t="n">
-        <v>646</v>
+        <v>996</v>
       </c>
       <c r="E41" t="n">
-        <v>10459</v>
+        <v>5758</v>
       </c>
       <c r="F41" t="n">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="G41" t="n">
-        <v>20.34</v>
+        <v>49.66</v>
       </c>
       <c r="H41" t="n">
-        <v>35.29</v>
+        <v>38.56</v>
       </c>
       <c r="I41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="b">
         <v>1</v>
       </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>11594</v>
+      </c>
+      <c r="L41" t="n">
+        <v>638</v>
+      </c>
       <c r="M41" t="n">
-        <v>1117489</v>
+        <v>704896</v>
       </c>
       <c r="N41" t="n">
-        <v>16.8</v>
+        <v>11.57</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Results from July 06, 2020 05:39:58 AM CT run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
@@ -1210,25 +1210,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44013</v>
+        <v>44016</v>
       </c>
       <c r="C16" t="n">
-        <v>107667</v>
+        <v>114993</v>
       </c>
       <c r="D16" t="n">
-        <v>3454</v>
+        <v>3487</v>
       </c>
       <c r="E16" t="n">
-        <v>2946</v>
+        <v>3112</v>
       </c>
       <c r="F16" t="n">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G16" t="n">
-        <v>4.6</v>
+        <v>4.67</v>
       </c>
       <c r="H16" t="n">
-        <v>11.37</v>
+        <v>11.3</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1237,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>63985</v>
+        <v>66661</v>
       </c>
       <c r="L16" t="n">
-        <v>3209</v>
+        <v>3240</v>
       </c>
       <c r="M16" t="n">
         <v>823987</v>

</xml_diff>

<commit_message>
Results from July 06, 2020 06:21:33 PM America/Chicago run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
@@ -522,16 +522,16 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C2" t="n">
-        <v>23133</v>
+        <v>23242</v>
       </c>
       <c r="D2" t="n">
         <v>680</v>
       </c>
       <c r="E2" t="n">
-        <v>2710</v>
+        <v>2721</v>
       </c>
       <c r="F2" t="n">
         <v>87</v>
@@ -572,10 +572,10 @@
         <v>44018</v>
       </c>
       <c r="C3" t="n">
-        <v>14751</v>
+        <v>15102</v>
       </c>
       <c r="D3" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -620,26 +620,26 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>213852</t>
+          <t>214061</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18583</t>
+          <t>18596</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33240</v>
+        <v>33265</v>
       </c>
       <c r="F4" t="n">
-        <v>5195</v>
+        <v>5199</v>
       </c>
       <c r="G4" t="n">
-        <v>30.17</v>
+        <v>30.16</v>
       </c>
       <c r="H4" t="n">
         <v>30.5</v>
@@ -651,10 +651,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>110192</v>
+        <v>110283</v>
       </c>
       <c r="L4" t="n">
-        <v>17034</v>
+        <v>17048</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -726,25 +726,25 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C6" t="n">
-        <v>51431</v>
+        <v>52155</v>
       </c>
       <c r="D6" t="n">
-        <v>646</v>
+        <v>653</v>
       </c>
       <c r="E6" t="n">
-        <v>10459</v>
+        <v>10640</v>
       </c>
       <c r="F6" t="n">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G6" t="n">
-        <v>20.34</v>
+        <v>20.4</v>
       </c>
       <c r="H6" t="n">
-        <v>35.29</v>
+        <v>35.38</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -773,21 +773,21 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>24952</t>
+          <t>25469</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>189</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>654</t>
+          <t>657</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44015</v>
+        <v>44018</v>
       </c>
       <c r="C8" t="n">
-        <v>16376</v>
+        <v>17152</v>
       </c>
       <c r="D8" t="n">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="E8" t="n">
-        <v>1607</v>
+        <v>1650</v>
       </c>
       <c r="F8" t="n">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="G8" t="n">
-        <v>14.06</v>
+        <v>14.14</v>
       </c>
       <c r="H8" t="n">
-        <v>15.72</v>
+        <v>4.14</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -853,10 +853,10 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>11432</v>
+        <v>11675</v>
       </c>
       <c r="L8" t="n">
-        <v>546</v>
+        <v>554</v>
       </c>
       <c r="M8" t="n">
         <v>354112</v>
@@ -1026,20 +1026,20 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C12" t="n">
-        <v>13256</v>
+        <v>13507</v>
       </c>
       <c r="D12" t="n">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E12" t="n">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>1.93</v>
+        <v>1.92</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="b">
@@ -1069,20 +1069,20 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C13" t="n">
-        <v>47011</v>
+        <v>48992</v>
       </c>
       <c r="D13" t="n">
-        <v>1043</v>
+        <v>1051</v>
       </c>
       <c r="E13" t="n">
-        <v>5798</v>
+        <v>5897</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>21.01</v>
+        <v>21.03</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>27600</v>
+        <v>28046</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
@@ -1114,20 +1114,20 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C14" t="n">
-        <v>14032</v>
+        <v>14407</v>
       </c>
       <c r="D14" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E14" t="n">
-        <v>1780</v>
+        <v>1842</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>23.96</v>
+        <v>24.03</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>7430</v>
+        <v>7664</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
@@ -1159,22 +1159,22 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C15" t="n">
-        <v>43450</v>
+        <v>44375</v>
       </c>
       <c r="D15" t="n">
         <v>984</v>
       </c>
       <c r="E15" t="n">
-        <v>15319</v>
+        <v>15481</v>
       </c>
       <c r="F15" t="n">
         <v>442</v>
       </c>
       <c r="G15" t="n">
-        <v>46.59</v>
+        <v>46.61</v>
       </c>
       <c r="H15" t="n">
         <v>46.48</v>
@@ -1186,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>32881</v>
+        <v>33213</v>
       </c>
       <c r="L15" t="n">
         <v>951</v>
@@ -1210,25 +1210,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="C16" t="n">
-        <v>114993</v>
+        <v>116570</v>
       </c>
       <c r="D16" t="n">
-        <v>3487</v>
+        <v>3534</v>
       </c>
       <c r="E16" t="n">
-        <v>3112</v>
+        <v>3170</v>
       </c>
       <c r="F16" t="n">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="G16" t="n">
-        <v>4.67</v>
+        <v>4.7</v>
       </c>
       <c r="H16" t="n">
-        <v>11.3</v>
+        <v>11.21</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1237,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>66661</v>
+        <v>67498</v>
       </c>
       <c r="L16" t="n">
-        <v>3240</v>
+        <v>3283</v>
       </c>
       <c r="M16" t="n">
         <v>823987</v>
@@ -1261,25 +1261,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C17" t="n">
-        <v>69632</v>
+        <v>69904</v>
       </c>
       <c r="D17" t="n">
-        <v>3118</v>
+        <v>3121</v>
       </c>
       <c r="E17" t="n">
-        <v>19953</v>
+        <v>20043</v>
       </c>
       <c r="F17" t="n">
-        <v>1258</v>
+        <v>1263</v>
       </c>
       <c r="G17" t="n">
-        <v>28.65</v>
+        <v>28.67</v>
       </c>
       <c r="H17" t="n">
-        <v>40.35</v>
+        <v>40.47</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1288,10 +1288,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>57047</v>
+        <v>57246</v>
       </c>
       <c r="L17" t="n">
-        <v>69602</v>
+        <v>69882</v>
       </c>
       <c r="M17" t="n">
         <v>1788090</v>
@@ -1312,25 +1312,25 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44015</v>
+        <v>44017</v>
       </c>
       <c r="C18" t="n">
-        <v>30674</v>
+        <v>31257</v>
       </c>
       <c r="D18" t="n">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="E18" t="n">
-        <v>14869</v>
+        <v>15110</v>
       </c>
       <c r="F18" t="n">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="G18" t="n">
-        <v>48.47</v>
+        <v>48.34</v>
       </c>
       <c r="H18" t="n">
-        <v>49.95</v>
+        <v>50.09</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -1359,16 +1359,16 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C19" t="n">
-        <v>87267</v>
+        <v>87705</v>
       </c>
       <c r="D19" t="n">
-        <v>6753</v>
+        <v>6754</v>
       </c>
       <c r="E19" t="n">
-        <v>11551</v>
+        <v>11603</v>
       </c>
       <c r="F19" t="n">
         <v>1426</v>
@@ -1386,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="K19" t="n">
-        <v>38441</v>
+        <v>38615</v>
       </c>
       <c r="L19" t="n">
         <v>6579</v>
@@ -1410,22 +1410,22 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C20" t="n">
-        <v>197076</v>
+        <v>203376</v>
       </c>
       <c r="D20" t="n">
-        <v>3731</v>
+        <v>3778</v>
       </c>
       <c r="E20" t="n">
-        <v>25942</v>
+        <v>26511</v>
       </c>
       <c r="F20" t="n">
-        <v>728</v>
+        <v>737</v>
       </c>
       <c r="G20" t="n">
-        <v>13.16</v>
+        <v>13.04</v>
       </c>
       <c r="H20" t="n">
         <v>19.51</v>
@@ -1457,10 +1457,10 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C21" t="n">
-        <v>1212</v>
+        <v>1249</v>
       </c>
       <c r="D21" t="n">
         <v>23</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="b">
@@ -1500,22 +1500,22 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C22" t="n">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="D22" t="n">
         <v>56</v>
       </c>
       <c r="E22" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>10.31</v>
+        <v>10.44</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>1213</v>
+        <v>1217</v>
       </c>
       <c r="L22" t="n">
         <v>56</v>
@@ -1551,25 +1551,25 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C23" t="n">
-        <v>34065</v>
+        <v>34257</v>
       </c>
       <c r="D23" t="n">
-        <v>1701</v>
+        <v>1691</v>
       </c>
       <c r="E23" t="n">
         <v>1809</v>
       </c>
       <c r="F23" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G23" t="n">
-        <v>6.45</v>
+        <v>6.42</v>
       </c>
       <c r="H23" t="n">
-        <v>6.78</v>
+        <v>6.76</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
@@ -1578,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>28039</v>
+        <v>28159</v>
       </c>
       <c r="L23" t="n">
-        <v>1638</v>
+        <v>1628</v>
       </c>
       <c r="M23" t="n">
         <v>227938</v>
@@ -1602,22 +1602,22 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C24" t="n">
-        <v>19929</v>
+        <v>20046</v>
       </c>
       <c r="D24" t="n">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E24" t="n">
-        <v>1180</v>
+        <v>1184</v>
       </c>
       <c r="F24" t="n">
         <v>21</v>
       </c>
       <c r="G24" t="n">
-        <v>7.66</v>
+        <v>7.65</v>
       </c>
       <c r="H24" t="n">
         <v>7.72</v>
@@ -1629,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>15406</v>
+        <v>15470</v>
       </c>
       <c r="L24" t="n">
         <v>272</v>
@@ -1653,25 +1653,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C25" t="n">
-        <v>65792</v>
+        <v>66089</v>
       </c>
       <c r="D25" t="n">
-        <v>5894</v>
+        <v>5897</v>
       </c>
       <c r="E25" t="n">
-        <v>19942</v>
+        <v>19987</v>
       </c>
       <c r="F25" t="n">
         <v>2358</v>
       </c>
       <c r="G25" t="n">
-        <v>30.31</v>
+        <v>30.24</v>
       </c>
       <c r="H25" t="n">
-        <v>40.01</v>
+        <v>39.99</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1700,25 +1700,25 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="C26" t="n">
-        <v>260155</v>
+        <v>271684</v>
       </c>
       <c r="D26" t="n">
-        <v>6264</v>
+        <v>6300</v>
       </c>
       <c r="E26" t="n">
-        <v>7432</v>
+        <v>7693</v>
       </c>
       <c r="F26" t="n">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="G26" t="n">
         <v>4.3</v>
       </c>
       <c r="H26" t="n">
-        <v>9.300000000000001</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1727,10 +1727,10 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>171792</v>
+        <v>177012</v>
       </c>
       <c r="L26" t="n">
-        <v>6163</v>
+        <v>6227</v>
       </c>
       <c r="M26" t="n">
         <v>2267875</v>
@@ -1751,25 +1751,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C27" t="n">
-        <v>48008</v>
+        <v>48331</v>
       </c>
       <c r="D27" t="n">
-        <v>2500</v>
+        <v>2505</v>
       </c>
       <c r="E27" t="n">
-        <v>5769</v>
+        <v>5798</v>
       </c>
       <c r="F27" t="n">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G27" t="n">
-        <v>12.02</v>
+        <v>12</v>
       </c>
       <c r="H27" t="n">
-        <v>14.48</v>
+        <v>14.49</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -1798,10 +1798,10 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C28" t="n">
-        <v>1138</v>
+        <v>1166</v>
       </c>
       <c r="D28" t="n">
         <v>16</v>
@@ -1813,7 +1813,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1.26</v>
+        <v>1.23</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>1982</v>
+        <v>2026</v>
       </c>
       <c r="L28" t="n">
         <v>32</v>
@@ -1849,22 +1849,22 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C29" t="n">
-        <v>31577</v>
+        <v>32061</v>
       </c>
       <c r="D29" t="n">
         <v>796</v>
       </c>
       <c r="E29" t="n">
-        <v>5412</v>
+        <v>5487</v>
       </c>
       <c r="F29" t="n">
         <v>188</v>
       </c>
       <c r="G29" t="n">
-        <v>19.08</v>
+        <v>19.04</v>
       </c>
       <c r="H29" t="n">
         <v>23.95</v>
@@ -1876,7 +1876,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>28371</v>
+        <v>28819</v>
       </c>
       <c r="L29" t="n">
         <v>785</v>
@@ -1900,25 +1900,25 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C30" t="n">
-        <v>95516</v>
+        <v>97064</v>
       </c>
       <c r="D30" t="n">
-        <v>2860</v>
+        <v>2878</v>
       </c>
       <c r="E30" t="n">
-        <v>26475</v>
+        <v>26887</v>
       </c>
       <c r="F30" t="n">
-        <v>1352</v>
+        <v>1357</v>
       </c>
       <c r="G30" t="n">
-        <v>27.72</v>
+        <v>27.7</v>
       </c>
       <c r="H30" t="n">
-        <v>47.27</v>
+        <v>47.15</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -2045,22 +2045,22 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C33" t="n">
-        <v>12128</v>
+        <v>12293</v>
       </c>
       <c r="D33" t="n">
         <v>512</v>
       </c>
       <c r="E33" t="n">
-        <v>3124</v>
+        <v>3148</v>
       </c>
       <c r="F33" t="n">
         <v>131</v>
       </c>
       <c r="G33" t="n">
-        <v>25.76</v>
+        <v>25.61</v>
       </c>
       <c r="H33" t="n">
         <v>25.59</v>
@@ -2092,20 +2092,20 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C34" t="n">
-        <v>3415</v>
+        <v>3423</v>
       </c>
       <c r="D34" t="n">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E34" t="n">
         <v>803</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>26.65</v>
+        <v>26.52</v>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="b">
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="K34" t="n">
-        <v>3013</v>
+        <v>3028</v>
       </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
@@ -2137,25 +2137,25 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C35" t="n">
-        <v>72983</v>
+        <v>74529</v>
       </c>
       <c r="D35" t="n">
-        <v>1396</v>
+        <v>1398</v>
       </c>
       <c r="E35" t="n">
-        <v>11722</v>
+        <v>11900</v>
       </c>
       <c r="F35" t="n">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G35" t="n">
-        <v>23.71</v>
+        <v>23.78</v>
       </c>
       <c r="H35" t="n">
-        <v>33.04</v>
+        <v>33.06</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -2164,10 +2164,10 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>49433</v>
+        <v>50048</v>
       </c>
       <c r="L35" t="n">
-        <v>1347</v>
+        <v>1349</v>
       </c>
       <c r="M35" t="n">
         <v>2179622</v>
@@ -2188,25 +2188,25 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C36" t="n">
-        <v>147251</v>
+        <v>147865</v>
       </c>
       <c r="D36" t="n">
-        <v>7020</v>
+        <v>7026</v>
       </c>
       <c r="E36" t="n">
-        <v>24691</v>
+        <v>24783</v>
       </c>
       <c r="F36" t="n">
         <v>1958</v>
       </c>
       <c r="G36" t="n">
-        <v>16.77</v>
+        <v>16.76</v>
       </c>
       <c r="H36" t="n">
-        <v>27.89</v>
+        <v>27.87</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -2235,25 +2235,25 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C37" t="n">
-        <v>7733</v>
+        <v>8052</v>
       </c>
       <c r="D37" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E37" t="n">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F37" t="n">
         <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>1.47</v>
+        <v>1.49</v>
       </c>
       <c r="H37" t="n">
-        <v>1.09</v>
+        <v>1.06</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -2282,25 +2282,25 @@
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C38" t="n">
-        <v>38136</v>
+        <v>38569</v>
       </c>
       <c r="D38" t="n">
-        <v>1471</v>
+        <v>1474</v>
       </c>
       <c r="E38" t="n">
-        <v>7861</v>
+        <v>7928</v>
       </c>
       <c r="F38" t="n">
         <v>125</v>
       </c>
       <c r="G38" t="n">
-        <v>20.61</v>
+        <v>20.56</v>
       </c>
       <c r="H38" t="n">
-        <v>8.5</v>
+        <v>8.48</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -2329,19 +2329,19 @@
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C39" t="n">
-        <v>109974</v>
+        <v>110137</v>
       </c>
       <c r="D39" t="n">
-        <v>8183</v>
+        <v>8198</v>
       </c>
       <c r="E39" t="n">
-        <v>10357</v>
+        <v>10370</v>
       </c>
       <c r="F39" t="n">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="G39" t="n">
         <v>9.42</v>
@@ -2376,25 +2376,25 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C40" t="n">
-        <v>12213</v>
+        <v>12436</v>
       </c>
       <c r="D40" t="n">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E40" t="n">
-        <v>3517</v>
+        <v>3592</v>
       </c>
       <c r="F40" t="n">
         <v>143</v>
       </c>
       <c r="G40" t="n">
-        <v>31.08</v>
+        <v>31.12</v>
       </c>
       <c r="H40" t="n">
-        <v>40.28</v>
+        <v>40.17</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -2403,10 +2403,10 @@
         <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>11317</v>
+        <v>11541</v>
       </c>
       <c r="L40" t="n">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M40" t="n">
         <v>252321</v>

</xml_diff>

<commit_message>
Results from July 06, 2020 09:21:49 PM America/Chicago run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -880,22 +880,22 @@
         <v>44018</v>
       </c>
       <c r="C9" t="n">
-        <v>23814</v>
+        <v>24253</v>
       </c>
       <c r="D9" t="n">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E9" t="n">
-        <v>5169</v>
+        <v>5239</v>
       </c>
       <c r="F9" t="n">
         <v>70</v>
       </c>
       <c r="G9" t="n">
-        <v>25.26</v>
+        <v>25.23</v>
       </c>
       <c r="H9" t="n">
-        <v>25.55</v>
+        <v>25.18</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -904,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>20467</v>
+        <v>20762</v>
       </c>
       <c r="L9" t="n">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M9" t="n">
         <v>460970</v>
@@ -928,22 +928,22 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C10" t="n">
-        <v>16726</v>
+        <v>17000</v>
       </c>
       <c r="D10" t="n">
         <v>387</v>
       </c>
       <c r="E10" t="n">
-        <v>606</v>
+        <v>615</v>
       </c>
       <c r="F10" t="n">
         <v>13</v>
       </c>
       <c r="G10" t="n">
-        <v>4.56</v>
+        <v>4.55</v>
       </c>
       <c r="H10" t="n">
         <v>3.4</v>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>13303</v>
+        <v>13514</v>
       </c>
       <c r="L10" t="n">
         <v>382</v>
@@ -1947,16 +1947,16 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C31" t="n">
-        <v>35898</v>
+        <v>36985</v>
       </c>
       <c r="D31" t="n">
-        <v>1359</v>
+        <v>1370</v>
       </c>
       <c r="E31" t="n">
-        <v>1436</v>
+        <v>1455</v>
       </c>
       <c r="F31" t="n">
         <v>45</v>
@@ -1974,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>26150</v>
+        <v>26515</v>
       </c>
       <c r="L31" t="n">
         <v>1301</v>
@@ -2471,6 +2471,39 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="n">
+        <v>109911</v>
+      </c>
+      <c r="N42" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "Update Dockerfile""
Reverting commit 64935f95ac09ed562fe1053233ba6d040d55759c rather than
editing it out of history so future pushes will merge this.
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-06.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -880,22 +880,22 @@
         <v>44018</v>
       </c>
       <c r="C9" t="n">
-        <v>23814</v>
+        <v>24253</v>
       </c>
       <c r="D9" t="n">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="E9" t="n">
-        <v>5169</v>
+        <v>5239</v>
       </c>
       <c r="F9" t="n">
         <v>70</v>
       </c>
       <c r="G9" t="n">
-        <v>25.26</v>
+        <v>25.23</v>
       </c>
       <c r="H9" t="n">
-        <v>25.55</v>
+        <v>25.18</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -904,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>20467</v>
+        <v>20762</v>
       </c>
       <c r="L9" t="n">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M9" t="n">
         <v>460970</v>
@@ -928,22 +928,22 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C10" t="n">
-        <v>16726</v>
+        <v>17000</v>
       </c>
       <c r="D10" t="n">
         <v>387</v>
       </c>
       <c r="E10" t="n">
-        <v>606</v>
+        <v>615</v>
       </c>
       <c r="F10" t="n">
         <v>13</v>
       </c>
       <c r="G10" t="n">
-        <v>4.56</v>
+        <v>4.55</v>
       </c>
       <c r="H10" t="n">
         <v>3.4</v>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>13303</v>
+        <v>13514</v>
       </c>
       <c r="L10" t="n">
         <v>382</v>
@@ -1947,16 +1947,16 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="C31" t="n">
-        <v>35898</v>
+        <v>36985</v>
       </c>
       <c r="D31" t="n">
-        <v>1359</v>
+        <v>1370</v>
       </c>
       <c r="E31" t="n">
-        <v>1436</v>
+        <v>1455</v>
       </c>
       <c r="F31" t="n">
         <v>45</v>
@@ -1974,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>26150</v>
+        <v>26515</v>
       </c>
       <c r="L31" t="n">
         <v>1301</v>
@@ -2471,6 +2471,39 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="n">
+        <v>109911</v>
+      </c>
+      <c r="N42" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>